<commit_message>
+ kombinasi status stamping
</commit_message>
<xml_diff>
--- a/Excel/2.1 Esign - Full API Services.xlsx
+++ b/Excel/2.1 Esign - Full API Services.xlsx
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="7065" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="7065" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="API Registrasi" sheetId="17" r:id="rId1"/>
     <sheet name="API Check Registrasi" sheetId="18" r:id="rId2"/>
     <sheet name="API Check Stamping Status" sheetId="19" r:id="rId3"/>
-    <sheet name="API Request Stamping" sheetId="20" r:id="rId4"/>
+    <sheet name="API Check Signing Status" sheetId="21" r:id="rId4"/>
+    <sheet name="API Request Stamping" sheetId="20" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="149">
   <si>
     <t>Status</t>
   </si>
@@ -427,18 +428,67 @@
   </si>
   <si>
     <t>"667_6"</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 not str dan 1 lagi proses upl doc</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 not str dan 1 lagi proses gen sdt</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 not str dan 1 lagi proses stm sdt</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 not str dan 1 lagi proses upl oss</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 not str dan 1 lagi proses upl con</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 not str dan 1 lagi proses sdt fin</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 sdt fin dan 1 lagi proses upl doc</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 sdt fin dan 1 lagi proses gent sdt</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 sdt fin dan 1 lagi proses stm sdt</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 sdt fin dan 1 lagi proses upl oss</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 sdt fin dan 1 lagi proses upl con</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 stm sdt dan 1 lagi proses sdt fin</t>
+  </si>
+  <si>
+    <t>Request dengan proses materai 52 atau 55 dan document ada 2 : 1 stm sdt dan 1 lagi proses gen sdt</t>
+  </si>
+  <si>
+    <t>""</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -592,51 +642,55 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="9" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="9" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2203,10 +2257,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W16"/>
+  <dimension ref="A1:AK16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -2216,100 +2270,158 @@
     <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="23" width="22" customWidth="1" collapsed="1"/>
+    <col min="24" max="32" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23">
+    <row r="1" spans="1:37">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-    </row>
-    <row r="2" spans="1:23" s="27" customFormat="1" ht="60">
+      <c r="T1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="27" customFormat="1" ht="60">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J2" t="s">
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
       <c r="T2" s="2"/>
       <c r="U2" s="2"/>
       <c r="V2" s="2"/>
-    </row>
-    <row r="3" spans="1:23" ht="78.75" customHeight="1">
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+    </row>
+    <row r="3" spans="1:37" ht="78.75" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -2367,12 +2479,52 @@
       <c r="S3" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-    </row>
-    <row r="4" spans="1:23">
+      <c r="T3" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG3" s="31"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+    </row>
+    <row r="4" spans="1:37">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2445,15 +2597,63 @@
         <v>0</v>
       </c>
       <c r="S4" s="2">
-        <f t="shared" ref="S4" si="3">COUNTIFS($A9:$A11,"*$*",S9:S11,"")</f>
-        <v>0</v>
-      </c>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-    </row>
-    <row r="5" spans="1:23">
+        <f t="shared" ref="S4:AF4" si="3">COUNTIFS($A9:$A11,"*$*",S9:S11,"")</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="V4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="W4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="X4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AE4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="2">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2477,8 +2677,17 @@
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-    </row>
-    <row r="6" spans="1:23" ht="14.25" customHeight="1">
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+    </row>
+    <row r="6" spans="1:37" ht="14.25" customHeight="1">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2502,8 +2711,17 @@
       <c r="U6" s="2"/>
       <c r="V6" s="2"/>
       <c r="W6" s="2"/>
-    </row>
-    <row r="7" spans="1:23" ht="14.25" customHeight="1">
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+    </row>
+    <row r="7" spans="1:37" ht="14.25" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2527,8 +2745,17 @@
       <c r="U7" s="2"/>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
-    </row>
-    <row r="8" spans="1:23">
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+    </row>
+    <row r="8" spans="1:37">
       <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
@@ -2551,11 +2778,20 @@
       <c r="R8" s="3"/>
       <c r="S8" s="4"/>
       <c r="T8" s="3"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-    </row>
-    <row r="9" spans="1:23">
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+    </row>
+    <row r="9" spans="1:37">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2613,12 +2849,47 @@
       <c r="S9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-    </row>
-    <row r="10" spans="1:23">
+      <c r="T9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="U9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="V9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="W9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="X9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37">
       <c r="A10" s="6" t="s">
         <v>10</v>
       </c>
@@ -2644,8 +2915,17 @@
       <c r="U10" s="7"/>
       <c r="V10" s="7"/>
       <c r="W10" s="7"/>
-    </row>
-    <row r="11" spans="1:23">
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+    </row>
+    <row r="11" spans="1:37">
       <c r="A11" s="1" t="s">
         <v>90</v>
       </c>
@@ -2703,12 +2983,47 @@
       <c r="S11" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="T11" s="1"/>
-      <c r="U11" s="1"/>
-      <c r="V11" s="1"/>
-      <c r="W11" s="5"/>
-    </row>
-    <row r="12" spans="1:23">
+      <c r="T11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="U11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="V11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="W11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="X11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AE11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF11" s="32" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37">
       <c r="A12" s="15" t="s">
         <v>69</v>
       </c>
@@ -2729,13 +3044,22 @@
       <c r="P12" s="15"/>
       <c r="Q12" s="15"/>
       <c r="R12" s="15"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-    </row>
-    <row r="13" spans="1:23">
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="15"/>
+      <c r="AF12" s="15"/>
+    </row>
+    <row r="13" spans="1:37">
       <c r="A13" s="11" t="s">
         <v>70</v>
       </c>
@@ -2793,12 +3117,47 @@
       <c r="S13" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
-      <c r="V13" s="1"/>
-      <c r="W13" s="1"/>
-    </row>
-    <row r="14" spans="1:23">
+      <c r="T13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="U13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="V13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="W13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="X13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF13" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37">
       <c r="A14" s="11" t="s">
         <v>71</v>
       </c>
@@ -2826,8 +3185,17 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
-    </row>
-    <row r="15" spans="1:23">
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+    </row>
+    <row r="15" spans="1:37">
       <c r="A15" s="24" t="s">
         <v>91</v>
       </c>
@@ -2885,12 +3253,47 @@
       <c r="S15" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="T15" s="1"/>
-      <c r="U15" s="1"/>
-      <c r="V15" s="1"/>
-      <c r="W15" s="1"/>
-    </row>
-    <row r="16" spans="1:23">
+      <c r="T15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="U15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="V15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="W15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="X15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF15" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37">
       <c r="A16" s="24" t="s">
         <v>92</v>
       </c>
@@ -2916,10 +3319,19 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B15:S15 B13:S13">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:AF13 B15:AF15">
       <formula1>"Yes, No"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2929,6 +3341,1091 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AK16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:AF2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="22" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="23" width="22" customWidth="1" collapsed="1"/>
+    <col min="24" max="32" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:37">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:37" s="27" customFormat="1" ht="60">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
+      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
+      <c r="V2" s="2"/>
+      <c r="W2" s="2"/>
+      <c r="X2" s="2"/>
+      <c r="Y2" s="2"/>
+      <c r="Z2" s="2"/>
+      <c r="AA2" s="2"/>
+      <c r="AB2" s="2"/>
+      <c r="AC2" s="2"/>
+      <c r="AD2" s="2"/>
+      <c r="AE2" s="2"/>
+      <c r="AF2" s="2"/>
+    </row>
+    <row r="3" spans="1:37" ht="78.75" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="K3" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="L3" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="M3" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="N3" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="O3" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="P3" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q3" s="23" t="s">
+        <v>122</v>
+      </c>
+      <c r="R3" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="S3" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="T3" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="AA3" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="AB3" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC3" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD3" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="AG3" s="31"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+    </row>
+    <row r="4" spans="1:37">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
+        <f t="shared" ref="B4:AF4" si="0">COUNTIFS($A9:$A11,"*$*",B9:B11,"")</f>
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="R4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="S4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="T4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="U4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="W4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="X4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Y4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Z4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AC4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AD4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AE4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AF4" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37">
+      <c r="A5" s="1"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="2"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="2"/>
+      <c r="T5" s="2"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+      <c r="AB5" s="1"/>
+      <c r="AC5" s="1"/>
+      <c r="AD5" s="1"/>
+      <c r="AE5" s="1"/>
+      <c r="AF5" s="1"/>
+    </row>
+    <row r="6" spans="1:37" ht="14.25" customHeight="1">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
+      <c r="Q6" s="2"/>
+      <c r="R6" s="2"/>
+      <c r="S6" s="2"/>
+      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
+      <c r="V6" s="2"/>
+      <c r="W6" s="2"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+      <c r="AB6" s="1"/>
+      <c r="AC6" s="1"/>
+      <c r="AD6" s="1"/>
+      <c r="AE6" s="1"/>
+      <c r="AF6" s="1"/>
+    </row>
+    <row r="7" spans="1:37" ht="14.25" customHeight="1">
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+      <c r="Q7" s="2"/>
+      <c r="R7" s="2"/>
+      <c r="S7" s="2"/>
+      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
+      <c r="V7" s="2"/>
+      <c r="W7" s="2"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+      <c r="AB7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+    </row>
+    <row r="8" spans="1:37">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+    </row>
+    <row r="9" spans="1:37">
+      <c r="A9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="O9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="U9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="V9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="W9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="X9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AA9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AD9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AE9" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="AF9" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+      <c r="AB10" s="7"/>
+      <c r="AC10" s="7"/>
+      <c r="AD10" s="7"/>
+      <c r="AE10" s="7"/>
+      <c r="AF10" s="7"/>
+    </row>
+    <row r="11" spans="1:37">
+      <c r="A11" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="H11" s="25" t="s">
+        <v>108</v>
+      </c>
+      <c r="I11" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="J11" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="K11" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="L11" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="M11" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="N11" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="O11" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="P11" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q11" s="24" t="s">
+        <v>123</v>
+      </c>
+      <c r="R11" s="24" t="s">
+        <v>125</v>
+      </c>
+      <c r="S11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="T11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="U11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="V11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="W11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="X11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="Y11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AA11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AC11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AD11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AE11" s="32" t="s">
+        <v>148</v>
+      </c>
+      <c r="AF11" s="32" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37">
+      <c r="A12" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
+      <c r="P12" s="15"/>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15"/>
+      <c r="S12" s="15"/>
+      <c r="T12" s="15"/>
+      <c r="U12" s="15"/>
+      <c r="V12" s="15"/>
+      <c r="W12" s="15"/>
+      <c r="X12" s="15"/>
+      <c r="Y12" s="15"/>
+      <c r="Z12" s="15"/>
+      <c r="AA12" s="15"/>
+      <c r="AB12" s="15"/>
+      <c r="AC12" s="15"/>
+      <c r="AD12" s="15"/>
+      <c r="AE12" s="15"/>
+      <c r="AF12" s="15"/>
+    </row>
+    <row r="13" spans="1:37">
+      <c r="A13" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="M13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="N13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="S13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="T13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="U13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="V13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="W13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="X13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE13" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF13" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37">
+      <c r="A14" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
+      <c r="AC14" s="1"/>
+      <c r="AD14" s="1"/>
+      <c r="AE14" s="1"/>
+      <c r="AF14" s="1"/>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="H15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="M15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="N15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="O15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="P15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="R15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="S15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="T15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="U15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="V15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="W15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="X15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AA15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AE15" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="AF15" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37">
+      <c r="A16" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AB16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AD16" s="1"/>
+      <c r="AE16" s="1"/>
+      <c r="AF16" s="1"/>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B13:AF13 B15:AF15">
+      <formula1>"Yes, No"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V16"/>
   <sheetViews>

</xml_diff>